<commit_message>
Atualização dos intervalos de alarme para temperatura
</commit_message>
<xml_diff>
--- a/Documentos/Intervalos_ArqComp.xlsx
+++ b/Documentos/Intervalos_ArqComp.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\Amonimous\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D0AC296-B09A-43A5-BB11-8BE78EB37CAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60BF3B-DED8-4D18-A077-B806B3DE04B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0451394B-AB32-49A0-ABFC-783F785DA76F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -284,12 +292,6 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,6 +304,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,7 +635,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D1" sqref="D1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,20 +650,20 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="H2" s="17" t="s">
+      <c r="F2" s="23"/>
+      <c r="H2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>4</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -669,14 +677,14 @@
       <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <f>F3+7.7</f>
         <v>11.7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="18">
         <f>I3+14.85</f>
         <v>14.85</v>
       </c>
@@ -685,7 +693,7 @@
       <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <f>F4+7.7</f>
         <v>19.399999999999999</v>
       </c>
@@ -702,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="10">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>7</v>
@@ -713,11 +721,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="20">
-        <v>27.9</v>
+      <c r="F7" s="18">
+        <v>27</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>6</v>

</xml_diff>